<commit_message>
docs: improve style of timing diagram
</commit_message>
<xml_diff>
--- a/FPGA/synth/RAM/doc/Excel/timing_diagram_ram_sp_wf.xlsx
+++ b/FPGA/synth/RAM/doc/Excel/timing_diagram_ram_sp_wf.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motchy\Documents\GitHub\code-fractions\FPGA\synth\ram\doc\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motchy\Documents\GitHub\code-fractions\FPGA\synth\RAM\doc\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A352F507-EDCC-4511-8347-90DA6A49A603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7389A33-88EF-4B54-93C6-D6233AE54485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{D9A37A3E-2F6F-469C-A47D-D0E2A71B6F48}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
   <si>
     <t>i_data</t>
     <phoneticPr fontId="1"/>
@@ -189,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -263,13 +263,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -324,13 +335,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
   </cellXfs>
@@ -659,7 +673,7 @@
   <dimension ref="A1:AA19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE12" sqref="AE12"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -675,7 +689,7 @@
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B3" t="s">
@@ -708,10 +722,10 @@
       <c r="AA3" s="5"/>
     </row>
     <row r="4" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="19"/>
+      <c r="A4" s="20"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="19"/>
+      <c r="A5" s="20"/>
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -742,10 +756,10 @@
       <c r="AA5" s="3"/>
     </row>
     <row r="6" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="19"/>
+      <c r="A7" s="20"/>
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -802,10 +816,10 @@
       <c r="AA7" s="2"/>
     </row>
     <row r="8" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="19"/>
+      <c r="A9" s="20"/>
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -838,10 +852,10 @@
       <c r="AA9" s="9"/>
     </row>
     <row r="10" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="19"/>
+      <c r="A10" s="20"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="19"/>
+      <c r="A11" s="20"/>
       <c r="B11" t="s">
         <v>0</v>
       </c>
@@ -898,70 +912,48 @@
       <c r="AA11" s="11"/>
     </row>
     <row r="12" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="B13" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="M13" s="2"/>
-      <c r="N13" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="O13" s="2"/>
-      <c r="P13" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="S13" s="2"/>
-      <c r="T13" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="U13" s="2"/>
-      <c r="V13" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="W13" s="2"/>
-      <c r="X13" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y13" s="2"/>
-      <c r="Z13" s="20" t="s">
-        <v>24</v>
-      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="21"/>
+      <c r="V13" s="21"/>
+      <c r="W13" s="21"/>
+      <c r="X13" s="21"/>
+      <c r="Y13" s="21"/>
+      <c r="Z13" s="21"/>
       <c r="AA13" s="2"/>
     </row>
     <row r="14" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="19"/>
+      <c r="A14" s="20"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
       <c r="B15" t="s">
         <v>1</v>
       </c>
@@ -1030,7 +1022,7 @@
       <c r="AA15" s="15"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B17" t="s">
@@ -1089,10 +1081,10 @@
       <c r="AA17" s="2"/>
     </row>
     <row r="18" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="18"/>
+      <c r="A18" s="19"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="18"/>
+      <c r="A19" s="19"/>
       <c r="B19" t="s">
         <v>9</v>
       </c>
@@ -1155,5 +1147,6 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>